<commit_message>
parameterize homeUrl for each environments.
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/Run.xlsx
+++ b/Automation/src/main/java/framework/test/Run.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/workspace/heal-qa-automation/Automation/src/main/java/framework/test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="520" yWindow="460" windowWidth="18800" windowHeight="14540" activeTab="1"/>
+    <workbookView xWindow="518" yWindow="458" windowWidth="18803" windowHeight="14543" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>Execute</t>
   </si>
@@ -76,9 +71,6 @@
     <t>screenResolution</t>
   </si>
   <si>
-    <t>url</t>
-  </si>
-  <si>
     <t>latest</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -87,10 +79,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>https://patient.qa.heal.com/login</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>browserName</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -152,21 +140,26 @@
     <t>addProfile</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>macOS 10.12</t>
+  </si>
+  <si>
+    <t>patient.qa.heal.com</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>baseUrl</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -181,13 +174,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -195,16 +188,8 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -244,24 +229,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="2">
+    <cellStyle name="已访问的超链接" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -566,19 +548,19 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A3" sqref="A3:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="22.1328125" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" customWidth="1"/>
+    <col min="5" max="5" width="36.1328125" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -598,9 +580,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>
@@ -609,9 +591,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -620,48 +602,48 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" t="s">
         <v>33</v>
       </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -676,17 +658,17 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.9"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="3"/>
+    <col min="3" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -694,85 +676,82 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -782,7 +761,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Completed critical (P0) test case
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/Run.xlsx
+++ b/Automation/src/main/java/framework/test/Run.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28502"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
   <workbookPr filterPrivacy="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="520" yWindow="460" windowWidth="18800" windowHeight="14540"/>
+    <workbookView xWindow="4780" yWindow="800" windowWidth="28820" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="43">
   <si>
     <t>Execute</t>
   </si>
@@ -55,104 +55,117 @@
     <t>Test Input</t>
   </si>
   <si>
+    <t>checkMenuLinksLoggedIn</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient.tests.LoginTest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>platform</t>
+  </si>
+  <si>
+    <t>version</t>
+  </si>
+  <si>
+    <t>screenResolution</t>
+  </si>
+  <si>
+    <t>latest</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1280x960</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>browserName</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>environment</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>USERNAME</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>ACCESS_KEY</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>qaheal</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>e14bb2d7-155b-4775-8978-9365c5b22012</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>patient.tests.ProfileTest</t>
+  </si>
+  <si>
+    <t>addInsuranceToExistingPatient</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>saucelab_url</t>
+  </si>
+  <si>
+    <t>@ondemand.saucelabs.com:443/wd/hub</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>editPayments</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>addProfile</t>
+  </si>
+  <si>
+    <t>macOS 10.12</t>
+  </si>
+  <si>
+    <t>baseUrl</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>loginWithValidCredentials</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>checkMenuLinksLoggedIn</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>patient.tests.LoginTest</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>platform</t>
-  </si>
-  <si>
-    <t>version</t>
-  </si>
-  <si>
-    <t>screenResolution</t>
-  </si>
-  <si>
-    <t>latest</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>1280x960</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>browserName</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>environment</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>N</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>bookVisit</t>
-  </si>
-  <si>
-    <t>USERNAME</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>ACCESS_KEY</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>qaheal</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>e14bb2d7-155b-4775-8978-9365c5b22012</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>patient.tests.ProfileTest</t>
-  </si>
-  <si>
-    <t>addInsuranceToExistingPatient</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>saucelab_url</t>
-  </si>
-  <si>
-    <t>@ondemand.saucelabs.com:443/wd/hub</t>
-  </si>
-  <si>
-    <t>local</t>
-  </si>
-  <si>
-    <t>editPayments</t>
-  </si>
-  <si>
-    <t>patient.tests.BookVisitTest</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>addProfile</t>
-  </si>
-  <si>
-    <t>macOS 10.12</t>
-  </si>
-  <si>
-    <t>baseUrl</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>patient-dev.heal.com</t>
+  </si>
+  <si>
+    <t>bookVisitWithCreditCard</t>
+  </si>
+  <si>
+    <t>patient.tests.VisitTest</t>
+  </si>
+  <si>
+    <t>BookVisitWithInsurance</t>
+  </si>
+  <si>
+    <t>BookVisitWith100PercentPromo</t>
+  </si>
+  <si>
+    <t>BookVisitWith50PercentPromo</t>
+  </si>
+  <si>
+    <t>cancelVisit</t>
+  </si>
+  <si>
+    <t>editProfile</t>
+  </si>
+  <si>
+    <t>patient.tests.PaymentsTest</t>
+  </si>
+  <si>
+    <t>patient.qa.heal.com</t>
   </si>
   <si>
     <t>N</t>
@@ -162,7 +175,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -196,6 +209,21 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -236,20 +264,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -589,71 +622,142 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" s="6" t="s">
         <v>9</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:F18">
+    <sortCondition ref="B2:B18"/>
+  </sortState>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -685,74 +789,74 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
use extent report page/test file update
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/Run.xlsx
+++ b/Automation/src/main/java/framework/test/Run.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="518" yWindow="458" windowWidth="18803" windowHeight="14543" activeTab="1"/>
+    <workbookView xWindow="518" yWindow="458" windowWidth="18803" windowHeight="14543"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -547,8 +547,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
@@ -593,7 +593,7 @@
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>10</v>
@@ -657,7 +657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added test rerun on failure
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/Run.xlsx
+++ b/Automation/src/main/java/framework/test/Run.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22380" yWindow="1240" windowWidth="28820" windowHeight="14540"/>
+    <workbookView xWindow="4780" yWindow="1240" windowWidth="28820" windowHeight="14540"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -588,7 +588,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix report with retry issue. read retryLimit from excel.
</commit_message>
<xml_diff>
--- a/Automation/src/main/java/framework/test/Run.xlsx
+++ b/Automation/src/main/java/framework/test/Run.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vahanmelikyan/Documents/workspace/heal-qa-automation/Automation/src/main/java/framework/test/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4780" yWindow="1240" windowWidth="28820" windowHeight="14540"/>
+    <workbookView xWindow="4778" yWindow="1238" windowWidth="28823" windowHeight="14543" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Scenarios" sheetId="1" r:id="rId1"/>
@@ -29,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="45">
   <si>
     <t>Execute</t>
   </si>
@@ -110,76 +105,86 @@
     <t>addInsuranceToExistingPatient</t>
   </si>
   <si>
+    <t>saucelab_url</t>
+  </si>
+  <si>
+    <t>@ondemand.saucelabs.com:443/wd/hub</t>
+  </si>
+  <si>
+    <t>local</t>
+  </si>
+  <si>
+    <t>editPayments</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>addProfile</t>
+  </si>
+  <si>
+    <t>macOS 10.12</t>
+  </si>
+  <si>
+    <t>baseUrl</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>loginWithValidCredentials</t>
+  </si>
+  <si>
+    <t>bookVisitWithCreditCard</t>
+  </si>
+  <si>
+    <t>patient.tests.VisitTest</t>
+  </si>
+  <si>
+    <t>BookVisitWithInsurance</t>
+  </si>
+  <si>
+    <t>BookVisitWith100PercentPromo</t>
+  </si>
+  <si>
+    <t>BookVisitWith50PercentPromo</t>
+  </si>
+  <si>
+    <t>cancelVisit</t>
+  </si>
+  <si>
+    <t>editProfile</t>
+  </si>
+  <si>
+    <t>patient.tests.PaymentsTest</t>
+  </si>
+  <si>
+    <t>patient.qa.heal.com</t>
+  </si>
+  <si>
+    <t>N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>saucelab_url</t>
-  </si>
-  <si>
-    <t>@ondemand.saucelabs.com:443/wd/hub</t>
-  </si>
-  <si>
-    <t>local</t>
-  </si>
-  <si>
-    <t>editPayments</t>
-  </si>
-  <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>addProfile</t>
-  </si>
-  <si>
-    <t>macOS 10.12</t>
-  </si>
-  <si>
-    <t>baseUrl</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>loginWithValidCredentials</t>
-  </si>
-  <si>
-    <t>bookVisitWithCreditCard</t>
-  </si>
-  <si>
-    <t>patient.tests.VisitTest</t>
-  </si>
-  <si>
-    <t>BookVisitWithInsurance</t>
-  </si>
-  <si>
-    <t>BookVisitWith100PercentPromo</t>
-  </si>
-  <si>
-    <t>BookVisitWith50PercentPromo</t>
-  </si>
-  <si>
-    <t>cancelVisit</t>
-  </si>
-  <si>
-    <t>editProfile</t>
-  </si>
-  <si>
-    <t>patient.tests.PaymentsTest</t>
-  </si>
-  <si>
-    <t>patient.qa.heal.com</t>
-  </si>
-  <si>
-    <t>N</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>retryLimit</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -194,13 +199,13 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -209,7 +214,7 @@
       <u/>
       <sz val="11"/>
       <color theme="11"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -217,14 +222,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="DengXian"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -280,10 +285,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="已访问的超链接" xfId="1" builtinId="9" hidden="1"/>
+    <cellStyle name="已访问的超链接" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="2" builtinId="8" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -584,23 +589,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A4" sqref="A4:A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <cols>
-    <col min="2" max="2" width="22.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="2" max="2" width="22.1328125" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" customWidth="1"/>
     <col min="4" max="4" width="27" customWidth="1"/>
-    <col min="5" max="5" width="36.1640625" customWidth="1"/>
+    <col min="5" max="5" width="36.1328125" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="14.65" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -620,20 +625,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B2" t="s">
         <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>9</v>
@@ -643,42 +648,42 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B5" t="s">
         <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B6" t="s">
         <v>21</v>
       </c>
       <c r="D6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B7" t="s">
         <v>21</v>
@@ -687,59 +692,59 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>42</v>
       </c>
       <c r="B8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" t="s">
         <v>34</v>
       </c>
-      <c r="D8" t="s">
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" t="s">
+    <row r="11" spans="1:6">
+      <c r="A11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>23</v>
-      </c>
-      <c r="B11" t="s">
-        <v>34</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="12" spans="1:6">
+      <c r="A12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
         <v>37</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>23</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -753,21 +758,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.1328125" defaultRowHeight="13.9"/>
   <cols>
     <col min="1" max="1" width="32.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.6640625" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="9.1640625" style="3"/>
+    <col min="3" max="16384" width="9.1328125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -775,31 +780,31 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -807,7 +812,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
@@ -815,15 +820,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -831,7 +836,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
@@ -839,12 +844,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -855,12 +868,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.9"/>
   <sheetData/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>